<commit_message>
Add A310-200/300 paints and update documentation
</commit_message>
<xml_diff>
--- a/documentation/Fixes and overviews.xlsx
+++ b/documentation/Fixes and overviews.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="251">
   <si>
     <t>Sound</t>
   </si>
@@ -841,16 +841,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -1135,14 +1133,14 @@
   <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,7 +1150,7 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1211,7 +1209,7 @@
       <c r="B8" t="s">
         <v>185</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1222,7 +1220,7 @@
       <c r="B9" t="s">
         <v>185</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1233,7 +1231,7 @@
       <c r="B10" t="s">
         <v>185</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1244,7 +1242,7 @@
       <c r="B11" t="s">
         <v>185</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1255,7 +1253,7 @@
       <c r="B12" t="s">
         <v>183</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>32234</v>
       </c>
     </row>
@@ -1266,7 +1264,7 @@
       <c r="B13" t="s">
         <v>183</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="1">
         <v>34516</v>
       </c>
     </row>
@@ -1274,6 +1272,12 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="B14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="1">
+        <v>30407</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1284,6 +1288,12 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
+      <c r="B16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" s="1">
+        <v>31413</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1330,12 +1340,12 @@
       <c r="B21" t="s">
         <v>183</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="6">
         <v>1989</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B22" t="s">
@@ -1352,7 +1362,7 @@
       <c r="B23" t="s">
         <v>183</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="6">
         <v>1994</v>
       </c>
     </row>
@@ -1363,7 +1373,7 @@
       <c r="B24" t="s">
         <v>183</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="1">
         <v>35400</v>
       </c>
     </row>
@@ -1374,7 +1384,7 @@
       <c r="B25" t="s">
         <v>183</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="1">
         <v>35886</v>
       </c>
     </row>
@@ -1385,7 +1395,7 @@
       <c r="B26" t="s">
         <v>183</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="1">
         <v>40360</v>
       </c>
     </row>
@@ -1427,7 +1437,7 @@
       <c r="B32" t="s">
         <v>185</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1449,7 +1459,7 @@
       <c r="B34" t="s">
         <v>185</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1460,7 +1470,7 @@
       <c r="B35" t="s">
         <v>185</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1471,7 +1481,7 @@
       <c r="B36" t="s">
         <v>185</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1492,7 +1502,7 @@
       <c r="B39" t="s">
         <v>185</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1503,7 +1513,7 @@
       <c r="B40" t="s">
         <v>185</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2009,7 +2019,7 @@
       <c r="B131" t="s">
         <v>183</v>
       </c>
-      <c r="C131" s="2">
+      <c r="C131" s="6">
         <v>1996</v>
       </c>
     </row>
@@ -2020,7 +2030,6 @@
       <c r="B132" t="s">
         <v>183</v>
       </c>
-      <c r="C132" s="5"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
@@ -2029,7 +2038,6 @@
       <c r="B133" t="s">
         <v>183</v>
       </c>
-      <c r="C133" s="5"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
@@ -2038,7 +2046,7 @@
       <c r="B134" t="s">
         <v>183</v>
       </c>
-      <c r="C134" s="4">
+      <c r="C134" s="1">
         <v>38047</v>
       </c>
     </row>
@@ -2049,7 +2057,7 @@
       <c r="B135" t="s">
         <v>183</v>
       </c>
-      <c r="C135" s="4">
+      <c r="C135" s="1">
         <v>38047</v>
       </c>
     </row>
@@ -2060,7 +2068,7 @@
       <c r="B136" t="s">
         <v>183</v>
       </c>
-      <c r="C136" s="4">
+      <c r="C136" s="1">
         <v>38047</v>
       </c>
     </row>
@@ -2071,7 +2079,7 @@
       <c r="B137" t="s">
         <v>183</v>
       </c>
-      <c r="C137" s="4">
+      <c r="C137" s="1">
         <v>38534</v>
       </c>
     </row>
@@ -2082,7 +2090,7 @@
       <c r="B138" t="s">
         <v>183</v>
       </c>
-      <c r="C138" s="4">
+      <c r="C138" s="1">
         <v>38534</v>
       </c>
     </row>
@@ -2093,7 +2101,7 @@
       <c r="B139" t="s">
         <v>183</v>
       </c>
-      <c r="C139" s="4">
+      <c r="C139" s="1">
         <v>38534</v>
       </c>
     </row>
@@ -2307,7 +2315,7 @@
       <c r="B180" t="s">
         <v>183</v>
       </c>
-      <c r="C180" s="4">
+      <c r="C180" s="1">
         <v>35309</v>
       </c>
     </row>
@@ -2366,7 +2374,7 @@
       <c r="A2" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="3">
         <v>100</v>
       </c>
       <c r="D2">
@@ -2747,7 +2755,7 @@
       <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="4">
         <v>70</v>
       </c>
       <c r="D35">
@@ -2857,7 +2865,7 @@
       <c r="A45" t="s">
         <v>202</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="5" t="s">
         <v>207</v>
       </c>
       <c r="D45">
@@ -2868,7 +2876,7 @@
       <c r="A46" t="s">
         <v>202</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="5" t="s">
         <v>208</v>
       </c>
       <c r="D46">
@@ -2879,7 +2887,7 @@
       <c r="A47" t="s">
         <v>202</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="5" t="s">
         <v>209</v>
       </c>
       <c r="D47">
@@ -2890,7 +2898,7 @@
       <c r="A48" t="s">
         <v>202</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="5" t="s">
         <v>210</v>
       </c>
       <c r="D48">
@@ -2912,7 +2920,7 @@
       <c r="A50" t="s">
         <v>202</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D50">
@@ -2923,7 +2931,7 @@
       <c r="A51" t="s">
         <v>202</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D51">
@@ -2934,7 +2942,7 @@
       <c r="A52" t="s">
         <v>202</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="5" t="s">
         <v>70</v>
       </c>
       <c r="D52">
@@ -2945,7 +2953,7 @@
       <c r="A53" t="s">
         <v>202</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D53">
@@ -2956,7 +2964,7 @@
       <c r="A54" t="s">
         <v>202</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C54">
@@ -2970,7 +2978,7 @@
       <c r="A55" t="s">
         <v>202</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D55">
@@ -2981,7 +2989,7 @@
       <c r="A56" t="s">
         <v>202</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C56">
@@ -2995,7 +3003,7 @@
       <c r="A57" t="s">
         <v>202</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="5" t="s">
         <v>76</v>
       </c>
       <c r="D57">
@@ -3006,7 +3014,7 @@
       <c r="A58" t="s">
         <v>202</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="5" t="s">
         <v>211</v>
       </c>
       <c r="D58">
@@ -3017,7 +3025,7 @@
       <c r="A59" t="s">
         <v>202</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D59">
@@ -3028,7 +3036,7 @@
       <c r="A60" t="s">
         <v>202</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="5" t="s">
         <v>212</v>
       </c>
       <c r="D60">
@@ -3039,7 +3047,7 @@
       <c r="A61" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D61">
@@ -3050,7 +3058,7 @@
       <c r="A62" t="s">
         <v>202</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="5" t="s">
         <v>88</v>
       </c>
       <c r="D62">
@@ -3061,7 +3069,7 @@
       <c r="A63" t="s">
         <v>202</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="5" t="s">
         <v>94</v>
       </c>
       <c r="D63">
@@ -3072,7 +3080,7 @@
       <c r="A64" t="s">
         <v>202</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D64">
@@ -3083,7 +3091,7 @@
       <c r="A65" t="s">
         <v>202</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="5" t="s">
         <v>213</v>
       </c>
       <c r="D65">
@@ -3094,7 +3102,7 @@
       <c r="A66" t="s">
         <v>202</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D66">
@@ -3105,7 +3113,7 @@
       <c r="A67" t="s">
         <v>202</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D67">
@@ -3116,7 +3124,7 @@
       <c r="A68" t="s">
         <v>202</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D68">
@@ -3127,7 +3135,7 @@
       <c r="A69" t="s">
         <v>202</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B69" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D69">
@@ -3138,7 +3146,7 @@
       <c r="A70" t="s">
         <v>202</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="5" t="s">
         <v>103</v>
       </c>
       <c r="D70">
@@ -3149,7 +3157,7 @@
       <c r="A71" t="s">
         <v>202</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C71">
@@ -3163,7 +3171,7 @@
       <c r="A72" t="s">
         <v>202</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="5" t="s">
         <v>214</v>
       </c>
       <c r="C72">
@@ -3177,7 +3185,7 @@
       <c r="A73" t="s">
         <v>202</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C73">
@@ -3191,7 +3199,7 @@
       <c r="A74" t="s">
         <v>202</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="5" t="s">
         <v>215</v>
       </c>
       <c r="D74">
@@ -3202,7 +3210,7 @@
       <c r="A75" t="s">
         <v>202</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="5" t="s">
         <v>110</v>
       </c>
       <c r="D75">
@@ -3213,7 +3221,7 @@
       <c r="A76" t="s">
         <v>202</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="5" t="s">
         <v>111</v>
       </c>
       <c r="D76">
@@ -3224,7 +3232,7 @@
       <c r="A77" t="s">
         <v>216</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="5" t="s">
         <v>175</v>
       </c>
       <c r="D77">
@@ -3246,7 +3254,7 @@
       <c r="A79" t="s">
         <v>217</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="5" t="s">
         <v>218</v>
       </c>
       <c r="D79">
@@ -3257,7 +3265,7 @@
       <c r="A80" t="s">
         <v>191</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="5" t="s">
         <v>219</v>
       </c>
       <c r="D80">
@@ -3268,7 +3276,7 @@
       <c r="A81" t="s">
         <v>191</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="5" t="s">
         <v>219</v>
       </c>
       <c r="D81">
@@ -3279,7 +3287,7 @@
       <c r="A82" t="s">
         <v>191</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="5" t="s">
         <v>220</v>
       </c>
       <c r="C82">
@@ -3293,7 +3301,7 @@
       <c r="A83" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="5" t="s">
         <v>221</v>
       </c>
       <c r="C83">
@@ -3307,7 +3315,7 @@
       <c r="A84" t="s">
         <v>191</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" s="5" t="s">
         <v>222</v>
       </c>
       <c r="C84">
@@ -3321,7 +3329,7 @@
       <c r="A85" t="s">
         <v>223</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B85" s="5" t="s">
         <v>164</v>
       </c>
       <c r="D85">
@@ -3332,7 +3340,7 @@
       <c r="A86" t="s">
         <v>223</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" s="5" t="s">
         <v>224</v>
       </c>
       <c r="D86">
@@ -3343,7 +3351,7 @@
       <c r="A87" t="s">
         <v>223</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="5" t="s">
         <v>165</v>
       </c>
       <c r="D87">
@@ -3354,7 +3362,7 @@
       <c r="A88" t="s">
         <v>223</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" s="5" t="s">
         <v>166</v>
       </c>
       <c r="D88">
@@ -3365,7 +3373,7 @@
       <c r="A89" t="s">
         <v>223</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" s="5" t="s">
         <v>225</v>
       </c>
       <c r="D89">
@@ -3376,7 +3384,7 @@
       <c r="A90" t="s">
         <v>223</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B90" s="5" t="s">
         <v>226</v>
       </c>
       <c r="D90">
@@ -3387,7 +3395,7 @@
       <c r="A91" t="s">
         <v>223</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="5" t="s">
         <v>227</v>
       </c>
       <c r="D91">
@@ -3398,7 +3406,7 @@
       <c r="A92" t="s">
         <v>223</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" s="5" t="s">
         <v>228</v>
       </c>
       <c r="D92">
@@ -3409,7 +3417,7 @@
       <c r="A93" t="s">
         <v>223</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="B93" s="5" t="s">
         <v>229</v>
       </c>
       <c r="D93">
@@ -3420,7 +3428,7 @@
       <c r="A94" t="s">
         <v>223</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B94" s="5" t="s">
         <v>230</v>
       </c>
       <c r="D94">
@@ -3431,7 +3439,7 @@
       <c r="A95" t="s">
         <v>223</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="5" t="s">
         <v>231</v>
       </c>
       <c r="D95">
@@ -3442,7 +3450,7 @@
       <c r="A96" t="s">
         <v>223</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B96" s="5" t="s">
         <v>232</v>
       </c>
       <c r="D96">
@@ -3453,7 +3461,7 @@
       <c r="A97" t="s">
         <v>223</v>
       </c>
-      <c r="B97" s="8" t="s">
+      <c r="B97" s="5" t="s">
         <v>233</v>
       </c>
       <c r="D97">
@@ -3464,7 +3472,7 @@
       <c r="A98" t="s">
         <v>223</v>
       </c>
-      <c r="B98" s="8" t="s">
+      <c r="B98" s="5" t="s">
         <v>234</v>
       </c>
       <c r="D98">
@@ -3475,7 +3483,7 @@
       <c r="A99" t="s">
         <v>235</v>
       </c>
-      <c r="B99" s="8" t="s">
+      <c r="B99" s="5" t="s">
         <v>236</v>
       </c>
       <c r="D99">
@@ -3486,7 +3494,7 @@
       <c r="A100" t="s">
         <v>235</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" s="5" t="s">
         <v>237</v>
       </c>
       <c r="D100">
@@ -3497,10 +3505,10 @@
       <c r="A101" t="s">
         <v>235</v>
       </c>
-      <c r="B101" s="8" t="s">
+      <c r="B101" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C101" s="7">
+      <c r="C101" s="4">
         <v>43</v>
       </c>
       <c r="D101">
@@ -3511,7 +3519,7 @@
       <c r="A102" t="s">
         <v>235</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="5" t="s">
         <v>239</v>
       </c>
       <c r="C102">
@@ -3525,7 +3533,7 @@
       <c r="A103" t="s">
         <v>235</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="B103" s="5" t="s">
         <v>240</v>
       </c>
       <c r="C103">
@@ -3539,7 +3547,7 @@
       <c r="A104" t="s">
         <v>235</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="5" t="s">
         <v>241</v>
       </c>
       <c r="C104">
@@ -3553,7 +3561,7 @@
       <c r="A105" t="s">
         <v>235</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="B105" s="5" t="s">
         <v>242</v>
       </c>
       <c r="C105">
@@ -3567,7 +3575,7 @@
       <c r="A106" t="s">
         <v>243</v>
       </c>
-      <c r="B106" s="8" t="s">
+      <c r="B106" s="5" t="s">
         <v>148</v>
       </c>
       <c r="C106">
@@ -3581,7 +3589,7 @@
       <c r="A107" t="s">
         <v>243</v>
       </c>
-      <c r="B107" s="8" t="s">
+      <c r="B107" s="5" t="s">
         <v>147</v>
       </c>
       <c r="D107">
@@ -3592,7 +3600,7 @@
       <c r="A108" t="s">
         <v>244</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B108" s="5" t="s">
         <v>149</v>
       </c>
       <c r="D108">
@@ -3603,7 +3611,7 @@
       <c r="A109" t="s">
         <v>223</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="B109" s="5" t="s">
         <v>167</v>
       </c>
       <c r="D109">
@@ -3614,7 +3622,7 @@
       <c r="A110" t="s">
         <v>223</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="B110" s="5" t="s">
         <v>168</v>
       </c>
       <c r="D110">
@@ -3625,7 +3633,7 @@
       <c r="A111" t="s">
         <v>223</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="B111" s="5" t="s">
         <v>169</v>
       </c>
       <c r="D111">
@@ -3636,7 +3644,7 @@
       <c r="A112" t="s">
         <v>223</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="B112" s="5" t="s">
         <v>170</v>
       </c>
       <c r="D112">
@@ -3647,7 +3655,7 @@
       <c r="A113" t="s">
         <v>223</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="B113" s="5" t="s">
         <v>171</v>
       </c>
       <c r="D113">
@@ -3658,7 +3666,7 @@
       <c r="A114" t="s">
         <v>223</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="B114" s="5" t="s">
         <v>172</v>
       </c>
       <c r="D114">
@@ -3669,7 +3677,7 @@
       <c r="A115" t="s">
         <v>223</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="B115" s="5" t="s">
         <v>173</v>
       </c>
       <c r="D115">
@@ -3680,7 +3688,7 @@
       <c r="A116" t="s">
         <v>223</v>
       </c>
-      <c r="B116" s="8" t="s">
+      <c r="B116" s="5" t="s">
         <v>174</v>
       </c>
       <c r="D116">
@@ -3691,7 +3699,7 @@
       <c r="A117" t="s">
         <v>191</v>
       </c>
-      <c r="B117" s="8" t="s">
+      <c r="B117" s="5" t="s">
         <v>245</v>
       </c>
       <c r="D117">
@@ -3702,7 +3710,7 @@
       <c r="A118" t="s">
         <v>191</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="B118" s="5" t="s">
         <v>246</v>
       </c>
       <c r="D118">
@@ -3713,7 +3721,7 @@
       <c r="A119" t="s">
         <v>191</v>
       </c>
-      <c r="B119" s="8" t="s">
+      <c r="B119" s="5" t="s">
         <v>247</v>
       </c>
       <c r="D119">
@@ -3724,7 +3732,7 @@
       <c r="A120" t="s">
         <v>248</v>
       </c>
-      <c r="B120" s="8" t="s">
+      <c r="B120" s="5" t="s">
         <v>178</v>
       </c>
       <c r="D120">
@@ -3735,10 +3743,10 @@
       <c r="A121" t="s">
         <v>248</v>
       </c>
-      <c r="B121" s="8" t="s">
+      <c r="B121" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C121" s="7">
+      <c r="C121" s="4">
         <v>76</v>
       </c>
       <c r="D121">
@@ -3749,7 +3757,7 @@
       <c r="A122" t="s">
         <v>248</v>
       </c>
-      <c r="B122" s="8" t="s">
+      <c r="B122" s="5" t="s">
         <v>249</v>
       </c>
       <c r="D122">
@@ -3760,7 +3768,7 @@
       <c r="A123" t="s">
         <v>248</v>
       </c>
-      <c r="B123" s="8" t="s">
+      <c r="B123" s="5" t="s">
         <v>250</v>
       </c>
       <c r="D123">

</xml_diff>

<commit_message>
Add Philippines B747-200 & B747-400
Add Philippines B747-200 & B747-400
Update documentation
Update intro years
Added capacity on 747-400M
</commit_message>
<xml_diff>
--- a/documentation/Fixes and overviews.xlsx
+++ b/documentation/Fixes and overviews.xlsx
@@ -280,9 +280,6 @@
     <t>B747-200</t>
   </si>
   <si>
-    <t>B747-200SUD</t>
-  </si>
-  <si>
     <t>B747-200F</t>
   </si>
   <si>
@@ -782,6 +779,9 @@
   </si>
   <si>
     <t>Tu154M</t>
+  </si>
+  <si>
+    <t>B747-200M</t>
   </si>
 </sst>
 </file>
@@ -1133,8 +1133,8 @@
   <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1159,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,7 +1167,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1175,7 +1175,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1191,7 +1191,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1199,7 +1199,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,10 +1207,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,10 +1218,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1229,10 +1229,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,10 +1240,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1251,7 +1251,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C12" s="1">
         <v>32234</v>
@@ -1262,7 +1262,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C13" s="1">
         <v>34516</v>
@@ -1273,7 +1273,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C14" s="1">
         <v>30407</v>
@@ -1289,7 +1289,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C16" s="1">
         <v>31413</v>
@@ -1305,7 +1305,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C18" s="1">
         <v>37271</v>
@@ -1316,7 +1316,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C19" s="1">
         <v>35180</v>
@@ -1327,7 +1327,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C20" s="1">
         <v>32230</v>
@@ -1338,7 +1338,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C21" s="6">
         <v>1989</v>
@@ -1346,10 +1346,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C22" s="1">
         <v>42394</v>
@@ -1360,7 +1360,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C23" s="6">
         <v>1994</v>
@@ -1371,7 +1371,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C24" s="1">
         <v>35400</v>
@@ -1382,7 +1382,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C25" s="1">
         <v>35886</v>
@@ -1393,7 +1393,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C26" s="1">
         <v>40360</v>
@@ -1404,7 +1404,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C27" s="1">
         <v>34640</v>
@@ -1435,10 +1435,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1446,7 +1446,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C33" s="1">
         <v>42019</v>
@@ -1457,10 +1457,10 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1468,10 +1468,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1479,10 +1479,10 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1500,10 +1500,10 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1511,10 +1511,10 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C77" s="1">
         <v>42877</v>
@@ -1723,162 +1723,177 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C82" s="1">
+        <v>25934</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>250</v>
+      </c>
+      <c r="C83" s="1">
+        <v>27030</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="C84" s="1">
+        <v>26299</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="C88" s="1">
+        <v>32548</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="C93" s="1">
+        <v>32752</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C111" s="1">
         <v>41860</v>
@@ -1886,55 +1901,55 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C121" s="1">
         <v>40526</v>
@@ -1942,10 +1957,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C122" s="1">
         <v>40526</v>
@@ -1953,10 +1968,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C123" s="1">
         <v>40526</v>
@@ -1964,60 +1979,60 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C131" s="6">
         <v>1996</v>
@@ -2025,26 +2040,26 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C134" s="1">
         <v>38047</v>
@@ -2052,10 +2067,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C135" s="1">
         <v>38047</v>
@@ -2063,10 +2078,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C136" s="1">
         <v>38047</v>
@@ -2074,10 +2089,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C137" s="1">
         <v>38534</v>
@@ -2085,10 +2100,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C138" s="1">
         <v>38534</v>
@@ -2096,10 +2111,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C139" s="1">
         <v>38534</v>
@@ -2107,213 +2122,213 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C180" s="1">
         <v>35309</v>
@@ -2321,12 +2336,12 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2358,21 +2373,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" t="s">
         <v>187</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>188</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>189</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B2" s="3">
         <v>100</v>
@@ -2383,7 +2398,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
@@ -2394,7 +2409,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
@@ -2405,7 +2420,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
@@ -2416,7 +2431,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6" t="s">
         <v>46</v>
@@ -2427,7 +2442,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
@@ -2438,10 +2453,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" t="s">
         <v>193</v>
-      </c>
-      <c r="B8" t="s">
-        <v>194</v>
       </c>
       <c r="D8">
         <v>29</v>
@@ -2449,10 +2464,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D9">
         <v>31</v>
@@ -2460,7 +2475,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
         <v>52</v>
@@ -2471,7 +2486,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -2482,7 +2497,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -2493,7 +2508,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -2504,7 +2519,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -2515,7 +2530,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2526,7 +2541,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -2537,7 +2552,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -2548,7 +2563,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
@@ -2559,10 +2574,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" t="s">
         <v>197</v>
-      </c>
-      <c r="B19" t="s">
-        <v>198</v>
       </c>
       <c r="D19">
         <v>54</v>
@@ -2570,7 +2585,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
@@ -2581,7 +2596,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -2592,7 +2607,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -2603,7 +2618,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
@@ -2614,10 +2629,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D24">
         <v>38</v>
@@ -2625,10 +2640,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D25">
         <v>45</v>
@@ -2636,7 +2651,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -2647,7 +2662,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -2658,7 +2673,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
@@ -2672,7 +2687,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -2683,7 +2698,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -2697,7 +2712,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -2711,7 +2726,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -2725,7 +2740,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
@@ -2736,7 +2751,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
@@ -2750,7 +2765,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B35" t="s">
         <v>37</v>
@@ -2764,7 +2779,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B36" t="s">
         <v>41</v>
@@ -2775,7 +2790,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
@@ -2786,10 +2801,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>201</v>
+      </c>
+      <c r="B38" t="s">
         <v>202</v>
-      </c>
-      <c r="B38" t="s">
-        <v>203</v>
       </c>
       <c r="D38">
         <v>44</v>
@@ -2797,10 +2812,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D39">
         <v>47</v>
@@ -2808,10 +2823,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D40">
         <v>47</v>
@@ -2819,10 +2834,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D41">
         <v>47</v>
@@ -2830,7 +2845,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B42" t="s">
         <v>60</v>
@@ -2841,7 +2856,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B43" t="s">
         <v>61</v>
@@ -2852,7 +2867,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B44" t="s">
         <v>63</v>
@@ -2863,10 +2878,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D45">
         <v>36</v>
@@ -2874,10 +2889,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D46">
         <v>40</v>
@@ -2885,10 +2900,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D47">
         <v>42</v>
@@ -2896,10 +2911,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D48">
         <v>44</v>
@@ -2907,7 +2922,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B49" t="s">
         <v>65</v>
@@ -2918,7 +2933,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>66</v>
@@ -2929,7 +2944,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>68</v>
@@ -2940,7 +2955,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>70</v>
@@ -2951,7 +2966,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>71</v>
@@ -2962,7 +2977,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>72</v>
@@ -2976,7 +2991,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>73</v>
@@ -2987,7 +3002,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>74</v>
@@ -3001,7 +3016,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>76</v>
@@ -3012,10 +3027,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D58">
         <v>56</v>
@@ -3023,7 +3038,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>79</v>
@@ -3034,10 +3049,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D60">
         <v>71</v>
@@ -3045,10 +3060,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D61">
         <v>71</v>
@@ -3056,10 +3071,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D62">
         <v>71</v>
@@ -3067,10 +3082,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D63">
         <v>76</v>
@@ -3078,10 +3093,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D64">
         <v>47</v>
@@ -3089,10 +3104,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D65">
         <v>47</v>
@@ -3100,10 +3115,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D66">
         <v>54</v>
@@ -3111,10 +3126,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D67">
         <v>49</v>
@@ -3122,10 +3137,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D68">
         <v>55</v>
@@ -3133,10 +3148,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D69">
         <v>55</v>
@@ -3144,10 +3159,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D70">
         <v>61</v>
@@ -3155,10 +3170,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C71">
         <v>62</v>
@@ -3169,10 +3184,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C72">
         <v>62</v>
@@ -3183,10 +3198,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C73">
         <v>70</v>
@@ -3197,10 +3212,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D74">
         <v>68</v>
@@ -3208,10 +3223,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D75">
         <v>57</v>
@@ -3219,10 +3234,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D76">
         <v>63</v>
@@ -3230,10 +3245,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D77">
         <v>31</v>
@@ -3241,7 +3256,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B78" t="s">
         <v>47</v>
@@ -3252,10 +3267,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>216</v>
+      </c>
+      <c r="B79" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="D79">
         <v>35</v>
@@ -3263,10 +3278,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D80">
         <v>27</v>
@@ -3274,10 +3289,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D81">
         <v>39</v>
@@ -3285,10 +3300,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C82">
         <v>37</v>
@@ -3299,10 +3314,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C83">
         <v>40</v>
@@ -3313,10 +3328,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C84">
         <v>44</v>
@@ -3327,10 +3342,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D85">
         <v>52</v>
@@ -3338,10 +3353,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>222</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="D86">
         <v>52</v>
@@ -3349,10 +3364,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D87">
         <v>52</v>
@@ -3360,10 +3375,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D88">
         <v>52</v>
@@ -3371,10 +3386,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D89">
         <v>43</v>
@@ -3382,10 +3397,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D90">
         <v>43</v>
@@ -3393,10 +3408,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D91">
         <v>43</v>
@@ -3404,10 +3419,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D92">
         <v>43</v>
@@ -3415,10 +3430,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D93">
         <v>43</v>
@@ -3426,10 +3441,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D94">
         <v>32</v>
@@ -3437,10 +3452,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D95">
         <v>32</v>
@@ -3448,10 +3463,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D96">
         <v>36</v>
@@ -3459,10 +3474,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D97">
         <v>38</v>
@@ -3470,10 +3485,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D98">
         <v>41</v>
@@ -3481,10 +3496,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>234</v>
+      </c>
+      <c r="B99" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>236</v>
       </c>
       <c r="D99">
         <v>26</v>
@@ -3492,10 +3507,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D100">
         <v>28</v>
@@ -3503,10 +3518,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C101" s="4">
         <v>43</v>
@@ -3517,10 +3532,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C102">
         <v>40</v>
@@ -3531,10 +3546,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C103">
         <v>41</v>
@@ -3545,10 +3560,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C104">
         <v>45</v>
@@ -3559,10 +3574,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C105">
         <v>47</v>
@@ -3573,10 +3588,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C106">
         <v>44</v>
@@ -3587,10 +3602,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D107">
         <v>31</v>
@@ -3598,10 +3613,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D108">
         <v>53</v>
@@ -3609,10 +3624,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D109">
         <v>62</v>
@@ -3620,10 +3635,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D110">
         <v>62</v>
@@ -3631,10 +3646,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D111">
         <v>45</v>
@@ -3642,10 +3657,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D112">
         <v>45</v>
@@ -3653,10 +3668,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D113">
         <v>45</v>
@@ -3664,10 +3679,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D114">
         <v>40</v>
@@ -3675,10 +3690,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D115">
         <v>45</v>
@@ -3686,10 +3701,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D116">
         <v>47</v>
@@ -3697,10 +3712,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D117">
         <v>22</v>
@@ -3708,10 +3723,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D118">
         <v>26</v>
@@ -3719,10 +3734,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D119">
         <v>33</v>
@@ -3730,10 +3745,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D120">
         <v>37</v>
@@ -3741,10 +3756,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C121" s="4">
         <v>76</v>
@@ -3755,10 +3770,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>247</v>
+      </c>
+      <c r="B122" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>249</v>
       </c>
       <c r="D122">
         <v>48</v>
@@ -3766,10 +3781,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D123">
         <v>48</v>

</xml_diff>

<commit_message>
Update docs and lng files
</commit_message>
<xml_diff>
--- a/documentation/Fixes and overviews.xlsx
+++ b/documentation/Fixes and overviews.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'AC Lenght'!$A$1:$D$123</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sound Fix'!$A$1:$C$182</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sound Fix'!$A$1:$C$171</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="239">
   <si>
     <t>Sound</t>
   </si>
@@ -58,18 +58,6 @@
     <t>72-500</t>
   </si>
   <si>
-    <t>A300B2</t>
-  </si>
-  <si>
-    <t>A300B4</t>
-  </si>
-  <si>
-    <t>A300F4</t>
-  </si>
-  <si>
-    <t>A300-600</t>
-  </si>
-  <si>
     <t>A300-600R</t>
   </si>
   <si>
@@ -127,33 +115,15 @@
     <t>A340-600</t>
   </si>
   <si>
-    <t>A350-800</t>
-  </si>
-  <si>
     <t>A350-900</t>
   </si>
   <si>
-    <t>A350-900R</t>
-  </si>
-  <si>
-    <t>A350-900F</t>
-  </si>
-  <si>
     <t>A350-1000</t>
   </si>
   <si>
     <t>A380-800</t>
   </si>
   <si>
-    <t>A380-800F</t>
-  </si>
-  <si>
-    <t>A380-900</t>
-  </si>
-  <si>
-    <t>A380-900F</t>
-  </si>
-  <si>
     <t>An124</t>
   </si>
   <si>
@@ -265,15 +235,9 @@
     <t>B737MAX 8</t>
   </si>
   <si>
-    <t>B747SP</t>
-  </si>
-  <si>
     <t>B747-100</t>
   </si>
   <si>
-    <t>B747-100SUD</t>
-  </si>
-  <si>
     <t>B747-100F</t>
   </si>
   <si>
@@ -298,12 +262,6 @@
     <t>B747-400D</t>
   </si>
   <si>
-    <t>B747-400F (BCF)</t>
-  </si>
-  <si>
-    <t>B747-400F/SCD</t>
-  </si>
-  <si>
     <t>B747-400ERF</t>
   </si>
   <si>
@@ -319,9 +277,6 @@
     <t>B757-200</t>
   </si>
   <si>
-    <t>B757-200PF</t>
-  </si>
-  <si>
     <t>B757-300</t>
   </si>
   <si>
@@ -355,9 +310,6 @@
     <t>B777-300ER</t>
   </si>
   <si>
-    <t>B777F</t>
-  </si>
-  <si>
     <t>B787-8</t>
   </si>
   <si>
@@ -782,6 +734,18 @@
   </si>
   <si>
     <t>B747-200M</t>
+  </si>
+  <si>
+    <t>B747-400F(SCD)</t>
+  </si>
+  <si>
+    <t>B747-400F(BCF)</t>
+  </si>
+  <si>
+    <t>B767-200ER</t>
+  </si>
+  <si>
+    <t>End date?</t>
   </si>
 </sst>
 </file>
@@ -841,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -849,6 +813,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -1130,11 +1095,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:D171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1108,7 @@
     <col min="3" max="3" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1154,205 +1119,217 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="C8" s="1">
+        <v>32234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="C9" s="1">
+        <v>34516</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="C10" s="1">
+        <v>30407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="C11" s="7">
+        <v>34335</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C12" s="1">
-        <v>32234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C13" s="1">
-        <v>34516</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C14" s="1">
-        <v>30407</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="1">
+        <v>35180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C16" s="1">
-        <v>31413</v>
+        <v>32230</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
+      <c r="B17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1989</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
+      <c r="A18" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C18" s="1">
-        <v>37271</v>
+        <v>42394</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
-      </c>
-      <c r="C19" s="1">
-        <v>35180</v>
+        <v>166</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1994</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C20" s="1">
-        <v>32230</v>
+        <v>35400</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="1">
+        <v>35886</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
-        <v>182</v>
-      </c>
-      <c r="C21" s="6">
-        <v>1989</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="B22" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C22" s="1">
-        <v>42394</v>
+        <v>40360</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1360,64 +1337,52 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C23" s="6">
-        <v>1994</v>
+        <v>166</v>
+      </c>
+      <c r="C23" s="1">
+        <v>34640</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>182</v>
-      </c>
-      <c r="C24" s="1">
-        <v>35400</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C25" s="1">
-        <v>35886</v>
-      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
-        <v>182</v>
-      </c>
-      <c r="C26" s="1">
-        <v>40360</v>
-      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
-        <v>182</v>
-      </c>
-      <c r="C27" s="1">
-        <v>34640</v>
-      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
+      <c r="B28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="1">
+        <v>42019</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1434,125 +1399,83 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
-        <v>184</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
-        <v>182</v>
-      </c>
-      <c r="C33" s="1">
-        <v>42019</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
-        <v>184</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
-        <v>184</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
-        <v>184</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B40" t="s">
-        <v>184</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1646,11 +1569,23 @@
       <c r="A66" t="s">
         <v>66</v>
       </c>
+      <c r="B66" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" s="1">
+        <v>39199</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
+      <c r="B67" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="1">
+        <v>42877</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
@@ -1658,7 +1593,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1666,693 +1601,628 @@
       <c r="A70" t="s">
         <v>70</v>
       </c>
+      <c r="C70" s="1">
+        <v>25934</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>234</v>
+      </c>
+      <c r="C71" s="1">
+        <v>27030</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>72</v>
+      <c r="B72" s="4"/>
+      <c r="C72" s="7">
+        <v>26299</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>76</v>
-      </c>
-      <c r="B76" t="s">
-        <v>182</v>
+        <v>75</v>
       </c>
       <c r="C76" s="1">
-        <v>39199</v>
+        <v>32548</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>77</v>
-      </c>
-      <c r="B77" t="s">
-        <v>182</v>
-      </c>
-      <c r="C77" s="1">
-        <v>42877</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>236</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>235</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="C81" s="1">
+        <v>32752</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>82</v>
-      </c>
-      <c r="C82" s="1">
-        <v>25934</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>250</v>
-      </c>
-      <c r="C83" s="1">
-        <v>27030</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
-      </c>
-      <c r="C84" s="1">
-        <v>26299</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
-      </c>
-      <c r="C88" s="1">
-        <v>32548</v>
+        <v>237</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
-      </c>
-      <c r="C93" s="1">
-        <v>32752</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>94</v>
+      </c>
+      <c r="B100" t="s">
+        <v>166</v>
+      </c>
+      <c r="C100" s="1">
+        <v>41860</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>104</v>
+      </c>
+      <c r="B110" t="s">
+        <v>166</v>
+      </c>
+      <c r="C110" s="1">
+        <v>40526</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B111" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C111" s="1">
-        <v>41860</v>
+        <v>40526</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>106</v>
+      </c>
+      <c r="B112" t="s">
+        <v>166</v>
+      </c>
+      <c r="C112" s="1">
+        <v>40526</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>107</v>
+      </c>
+      <c r="B113" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>108</v>
+      </c>
+      <c r="B114" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+      <c r="B115" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="B116" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="B117" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="B120" t="s">
+        <v>166</v>
+      </c>
+      <c r="C120" s="6">
+        <v>1996</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B121" t="s">
-        <v>182</v>
-      </c>
-      <c r="C121" s="1">
-        <v>40526</v>
+        <v>166</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B122" t="s">
-        <v>182</v>
-      </c>
-      <c r="C122" s="1">
-        <v>40526</v>
+        <v>166</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B123" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C123" s="1">
-        <v>40526</v>
+        <v>38047</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B124" t="s">
-        <v>185</v>
+        <v>166</v>
+      </c>
+      <c r="C124" s="1">
+        <v>38047</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B125" t="s">
-        <v>185</v>
+        <v>166</v>
+      </c>
+      <c r="C125" s="1">
+        <v>38047</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B126" t="s">
-        <v>185</v>
+        <v>166</v>
+      </c>
+      <c r="C126" s="1">
+        <v>38534</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B127" t="s">
-        <v>185</v>
+        <v>166</v>
+      </c>
+      <c r="C127" s="1">
+        <v>38534</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>122</v>
+      </c>
+      <c r="B128" t="s">
+        <v>166</v>
+      </c>
+      <c r="C128" s="1">
+        <v>38534</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>127</v>
       </c>
-      <c r="B128" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="B135" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>130</v>
       </c>
-      <c r="B131" t="s">
-        <v>182</v>
-      </c>
-      <c r="C131" s="6">
-        <v>1996</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>131</v>
       </c>
-      <c r="B132" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>132</v>
       </c>
-      <c r="B133" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>133</v>
       </c>
-      <c r="B134" t="s">
-        <v>182</v>
-      </c>
-      <c r="C134" s="1">
-        <v>38047</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>134</v>
       </c>
-      <c r="B135" t="s">
-        <v>182</v>
-      </c>
-      <c r="C135" s="1">
-        <v>38047</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>135</v>
       </c>
-      <c r="B136" t="s">
-        <v>182</v>
-      </c>
-      <c r="C136" s="1">
-        <v>38047</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>136</v>
       </c>
-      <c r="B137" t="s">
-        <v>182</v>
-      </c>
-      <c r="C137" s="1">
-        <v>38534</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>137</v>
       </c>
-      <c r="B138" t="s">
-        <v>182</v>
-      </c>
-      <c r="C138" s="1">
-        <v>38534</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>138</v>
       </c>
-      <c r="B139" t="s">
-        <v>182</v>
-      </c>
-      <c r="C139" s="1">
-        <v>38534</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>145</v>
       </c>
-      <c r="B146" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="B169" t="s">
+        <v>166</v>
+      </c>
+      <c r="C169" s="1">
+        <v>35309</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>179</v>
-      </c>
-      <c r="B180" t="s">
-        <v>182</v>
-      </c>
-      <c r="C180" s="1">
-        <v>35309</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>181</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C182"/>
+  <autoFilter ref="A1:C171"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2379,21 +2249,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="C1" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B2" s="3">
         <v>100</v>
@@ -2404,10 +2274,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>29</v>
@@ -2415,10 +2285,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>29</v>
@@ -2426,10 +2296,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>29</v>
@@ -2437,10 +2307,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>33</v>
@@ -2448,10 +2318,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>26</v>
@@ -2459,10 +2329,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="D8">
         <v>29</v>
@@ -2470,10 +2340,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="D9">
         <v>31</v>
@@ -2481,10 +2351,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D10">
         <v>31</v>
@@ -2492,7 +2362,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -2503,7 +2373,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -2514,7 +2384,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -2525,7 +2395,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -2536,7 +2406,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2547,7 +2417,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -2558,10 +2428,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>54</v>
@@ -2569,10 +2439,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D18">
         <v>54</v>
@@ -2580,10 +2450,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="D19">
         <v>54</v>
@@ -2591,10 +2461,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <v>47</v>
@@ -2602,10 +2472,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>47</v>
@@ -2613,10 +2483,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22">
         <v>32</v>
@@ -2624,10 +2494,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D23">
         <v>34</v>
@@ -2635,10 +2505,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B24" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="D24">
         <v>38</v>
@@ -2646,10 +2516,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B25" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="D25">
         <v>45</v>
@@ -2657,10 +2527,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D26">
         <v>59</v>
@@ -2668,10 +2538,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D27">
         <v>59</v>
@@ -2679,10 +2549,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C28">
         <v>69</v>
@@ -2693,10 +2563,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D29">
         <v>59</v>
@@ -2704,10 +2574,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C30">
         <v>69</v>
@@ -2718,10 +2588,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <v>72</v>
@@ -2732,10 +2602,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C32">
         <v>76</v>
@@ -2746,10 +2616,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D33">
         <v>74</v>
@@ -2757,10 +2627,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C34">
         <v>72</v>
@@ -2771,10 +2641,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C35" s="4">
         <v>70</v>
@@ -2785,10 +2655,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D36">
         <v>69</v>
@@ -2796,10 +2666,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D37">
         <v>84</v>
@@ -2807,10 +2677,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B38" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="D38">
         <v>44</v>
@@ -2818,10 +2688,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B39" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D39">
         <v>47</v>
@@ -2829,10 +2699,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B40" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="D40">
         <v>47</v>
@@ -2840,10 +2710,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B41" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D41">
         <v>47</v>
@@ -2851,10 +2721,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D42">
         <v>38</v>
@@ -2862,10 +2732,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D43">
         <v>41</v>
@@ -2873,10 +2743,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D44">
         <v>47</v>
@@ -2884,10 +2754,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="D45">
         <v>36</v>
@@ -2895,10 +2765,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="D46">
         <v>40</v>
@@ -2906,10 +2776,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="D47">
         <v>42</v>
@@ -2917,10 +2787,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="D48">
         <v>44</v>
@@ -2928,10 +2798,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D49">
         <v>29</v>
@@ -2939,10 +2809,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D50">
         <v>31</v>
@@ -2950,10 +2820,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D51">
         <v>33</v>
@@ -2961,10 +2831,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D52">
         <v>36</v>
@@ -2972,10 +2842,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D53">
         <v>31</v>
@@ -2983,10 +2853,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C54">
         <v>40</v>
@@ -2997,10 +2867,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D55">
         <v>34</v>
@@ -3008,10 +2878,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C56">
         <v>46</v>
@@ -3022,10 +2892,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D57">
         <v>42</v>
@@ -3033,10 +2903,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="D58">
         <v>56</v>
@@ -3044,10 +2914,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D59">
         <v>71</v>
@@ -3055,10 +2925,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="D60">
         <v>71</v>
@@ -3066,10 +2936,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D61">
         <v>71</v>
@@ -3077,10 +2947,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D62">
         <v>71</v>
@@ -3088,10 +2958,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D63">
         <v>76</v>
@@ -3099,10 +2969,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D64">
         <v>47</v>
@@ -3110,10 +2980,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="D65">
         <v>47</v>
@@ -3121,10 +2991,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D66">
         <v>54</v>
@@ -3132,10 +3002,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D67">
         <v>49</v>
@@ -3143,10 +3013,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D68">
         <v>55</v>
@@ -3154,10 +3024,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D69">
         <v>55</v>
@@ -3165,10 +3035,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D70">
         <v>61</v>
@@ -3176,10 +3046,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C71">
         <v>62</v>
@@ -3190,10 +3060,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="C72">
         <v>62</v>
@@ -3204,10 +3074,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C73">
         <v>70</v>
@@ -3218,10 +3088,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="D74">
         <v>68</v>
@@ -3229,10 +3099,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D75">
         <v>57</v>
@@ -3240,10 +3110,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="D76">
         <v>63</v>
@@ -3251,10 +3121,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="D77">
         <v>31</v>
@@ -3262,10 +3132,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B78" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D78">
         <v>62</v>
@@ -3273,10 +3143,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="D79">
         <v>35</v>
@@ -3284,10 +3154,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="D80">
         <v>27</v>
@@ -3295,10 +3165,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="D81">
         <v>39</v>
@@ -3306,10 +3176,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C82">
         <v>37</v>
@@ -3320,10 +3190,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="C83">
         <v>40</v>
@@ -3334,10 +3204,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="C84">
         <v>44</v>
@@ -3348,10 +3218,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="D85">
         <v>52</v>
@@ -3359,10 +3229,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="D86">
         <v>52</v>
@@ -3370,10 +3240,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="D87">
         <v>52</v>
@@ -3381,10 +3251,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="D88">
         <v>52</v>
@@ -3392,10 +3262,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="D89">
         <v>43</v>
@@ -3403,10 +3273,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="D90">
         <v>43</v>
@@ -3414,10 +3284,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="D91">
         <v>43</v>
@@ -3425,10 +3295,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="D92">
         <v>43</v>
@@ -3436,10 +3306,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="D93">
         <v>43</v>
@@ -3447,10 +3317,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="D94">
         <v>32</v>
@@ -3458,10 +3328,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="D95">
         <v>32</v>
@@ -3469,10 +3339,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="D96">
         <v>36</v>
@@ -3480,10 +3350,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="D97">
         <v>38</v>
@@ -3491,10 +3361,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="D98">
         <v>41</v>
@@ -3502,10 +3372,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="D99">
         <v>26</v>
@@ -3513,10 +3383,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="D100">
         <v>28</v>
@@ -3524,10 +3394,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="C101" s="4">
         <v>43</v>
@@ -3538,10 +3408,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="C102">
         <v>40</v>
@@ -3552,10 +3422,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="C103">
         <v>41</v>
@@ -3566,10 +3436,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="C104">
         <v>45</v>
@@ -3580,10 +3450,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="C105">
         <v>47</v>
@@ -3594,10 +3464,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C106">
         <v>44</v>
@@ -3608,10 +3478,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="D107">
         <v>31</v>
@@ -3619,10 +3489,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D108">
         <v>53</v>
@@ -3630,10 +3500,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="D109">
         <v>62</v>
@@ -3641,10 +3511,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="D110">
         <v>62</v>
@@ -3652,10 +3522,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="D111">
         <v>45</v>
@@ -3663,10 +3533,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="D112">
         <v>45</v>
@@ -3674,10 +3544,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="D113">
         <v>45</v>
@@ -3685,10 +3555,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D114">
         <v>40</v>
@@ -3696,10 +3566,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="D115">
         <v>45</v>
@@ -3707,10 +3577,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="D116">
         <v>47</v>
@@ -3718,10 +3588,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="D117">
         <v>22</v>
@@ -3729,10 +3599,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="D118">
         <v>26</v>
@@ -3740,10 +3610,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="D119">
         <v>33</v>
@@ -3751,10 +3621,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="D120">
         <v>37</v>
@@ -3762,10 +3632,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C121" s="4">
         <v>76</v>
@@ -3776,10 +3646,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="D122">
         <v>48</v>
@@ -3787,10 +3657,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="D123">
         <v>48</v>

</xml_diff>